<commit_message>
adding a lot fo stuff
</commit_message>
<xml_diff>
--- a/Scrapping_test/job.xlsx
+++ b/Scrapping_test/job.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G70"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -375,20 +375,10 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>salary</t>
+          <t>location</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>location</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>closed_date</t>
         </is>
@@ -397,229 +387,174 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Մատուցող / Մատուցողուհիներ</t>
+          <t>Technical Sales and Customer Support Agent</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Sorriso Cafe Gelateria</t>
+          <t>Piconet</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Restaurants, Food Services</t>
+          <t>Customer Support, Client Care</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>200000</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ոչ լրիվ աշխատանքային օր Ճկուն գրաֆիկ Ճանապարհածախս Համազգեստ Պաշտոնապես աշխատանքի հաշվառում Կարիերային առաջխաղացման հնարավորություն </t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>4/1/2019</t>
+          <t>4/29/2019</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Տնօրեն - Իրավաբան</t>
+          <t>Մատուցող / Մատուցողուհի</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Hydrocorporation</t>
+          <t>Man bevrijing</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Project, Program Management</t>
+          <t>Restaurants, Food Services</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>350000</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Բարձրագույն իրավաբանական կրթություն, Աշխատանքային փորձ կառավարման ոլորտում, Համակարգչային բազային գիտելիքներ (MC office), Լեզուների իմացությունը կդիտվի որպես առավելություն: </t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>4/1/2019</t>
+          <t>4/29/2019</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>SMM մասնագետ</t>
+          <t>Վաճառողուհի Գանձապահ</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Տիկո Հոլդինգ ՍՊԸ</t>
+          <t>Laura Ashley</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Marketing, Advertising, PR</t>
+          <t>Sales, Business Development</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>4/1/2019</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t xml:space="preserve">կրթությունը՝ բարձրագույն կրթություն մարքեթինգի, հանրային կապերի կամ հարակից որևէ ոլորտում (ցանկալի) աշխատանքային փորձը ցանկալի է  պարտադիր հմտություններ՝  ստեղծագործական և նորարարական մոտեցում աշխատանքին ցանկալի հմտություններ՝ գրաֆիկական դիզայնի ծրագրերի իմացություն (Photoshop, Corеl Draw և այլն) </t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>5/1/2019</t>
+          <t>5/29/2019</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Night Shift Receptionist</t>
+          <t>Ավտոփականագործ</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Bass Boutique Hotel</t>
+          <t>ՄԵԾ ԱՆԻՎ</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Tourism, Hospitality</t>
+          <t>Installation, Maintenance, Repair</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>3/30/2019</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>4/29/2019</t>
+          <t>Yerevan</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>5/29/2019</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Store Manager</t>
+          <t>Մենեջեր</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>EGO Concept Store</t>
+          <t>Solare LLC</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Customer Support, Client Care</t>
+          <t>Sales, Business Development</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>3/29/2019</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t xml:space="preserve">կոկիկ և ներկայանալի արտաքին գրագետ խոսք (անգլերեն և ռուսերեն լեզուների իմացությունը կդիտվի որպես առավելություն) համակարգչային տարրական գիտելիքներ բարձրագույն կամ միջին մասնագիտական կրթություն աշխատանքային փորձ սպասարկման ոլորտում հաճախորդների հետ բարեհամբույր հաղորդակցման ունակություն կարգապահություն, ազնվություն, ոչ կոնֆլիկտային բնավորություն ժպտալու և լավ տրամադրություն հաղորդելու պատրաստակամություն, նույնիսկ աշխատանքային օրվա վերջում </t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>4/29/2019</t>
+          <t>5/27/2019</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Վաճառող - Խորհրդատու</t>
+          <t>Գլխավոր Հաշվապահ</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Տիկո Հոլդինգ ՍՊԸ</t>
+          <t>Solare LLC</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Sales, Business Development</t>
+          <t>Accounting, Finance, Banking</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>100,000 + % վաճառքից</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Աշխատանքային փորձն ու դիմահարդարման հմտությունները ցանկալի են Նպատակասլացություն Պատասխանատվություն Հաղորդակցման հմտություններ Վաճառքի հմտություններ </t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>3/29/2019</t>
+          <t>5/27/2019</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Վաճառող - Խորհրդատու</t>
+          <t>Վաճառքի Մենեջեր</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Gioielli Boutique</t>
+          <t>NewPlast CJSC</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -629,34 +564,24 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>3/29/2019</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Բարձրագույն կրթություն, Սպասարկման ոլորտում աշխատանքային փորձը ցանկալի է, Ռուսերեն և անգլերեն լեզուների իմացություն, Համակարգչային բազային գիտելիքներ, Հաղորդակցման և թիմային աշխատանքի հմտություններ, Ճշտապահություն և պատասխանատվության զգացում, Նոր գիտելիքների և հմտությունների ձեռք բերելու  ցանկություն: </t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>4/28/2019</t>
+          <t>5/27/2019</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Ինժեներ - Նախագծող /Կոնստրուկտոր/</t>
+          <t>Ինժեներ  Էլեկտրոնշիկ</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>KMK LLC</t>
+          <t>NewPlast CJSC</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -666,293 +591,213 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>3/29/2019</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t xml:space="preserve">բարձրագույն, թերի բարձրագույն, միջին մասնագիտական կրթություն վստահ PC օգտվող: AUTOCAD / SolidWorks գիտելիքները; ուշադրություն; ճշգրտություն; պատասխանատվություն; ճշտապահություն; ռուսաց լեզվի իմացություն, տեխնիկական անգլերենի իմացությունը ցանկալի է: </t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Moscow region, Klin city, Russia</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>4/28/2019</t>
+          <t>5/27/2019</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Փրկարար</t>
+          <t>Վաճառող - Մատուցող</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Վալենսիա ՀՁ ՍՊԸ</t>
+          <t>Baguette &amp; Co</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Restaurants, Food Services</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>3/29/2019</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Սեռ՝ արական, իգական Պարտադիր լողալու կարողությամբ Տարիք՝ 18-35տ Բարձրագույն մասնագիտական կրթությունը ցանկալի է / լողի բաժին, ջրացատկ/ Ցանկալի է ունենալ լողորդի որակավորում՝ սերտիֆիկատ, դիպլոմ Ուշադրություն, զգոնություն ջրայգում հանգստացող հաճախորդների նկատմանբ </t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>4/5/2019</t>
+          <t>5/26/2019</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Տեխնիկական Վերահսկողության Մասնագետ</t>
+          <t>Վաճառքի Բաժնի Աշխատակից</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ARCON</t>
+          <t>8778 Հայաստան Տեղեկատու</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Production, Operations</t>
+          <t>Sales, Business Development</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>3/29/2019</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t xml:space="preserve">1-3 տարվա արտադրության աշխատանքային փորձ, Ռուսաց լեզվի վարժ տիրապետում, Բարձրագույն կամ միջին մասնագիտական տեխնիկական կրթություն, MS Office- ի իմացություն, 1C- ի իմացությունը ողջունելի է, Ավտոմեքենայի առկայությունը ողջունելի է, Ծրագրերի կառավարման փորձ, Վերլուծական միտք, Պատասխանատվության զգացում, Հաստատակամություն, Ջանասիրություն, Բազմակողմանի աշխատանք վարելու ունակություն, Սթրեսակայունություն: </t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>4/28/2019</t>
+          <t>4/26/2019</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Անշարժ Գույքի Գործակալ</t>
+          <t>Խորհրդատու Վաճառողուհի</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Alex-R</t>
+          <t>ԿՈՆՏԵ ԷԼԵԳԱՆՏ ՍՊԸ</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Real Estate</t>
+          <t>Sales, Business Development</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>120000</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t xml:space="preserve">Մեքենա վարելու ունակություն, Համակարգչից վարժ օգտվելու ունակություն, Թիմային աշխատանքի հմտություններ, Հաճախորդների հետ շփման, արագ կողմնորոշման ունակություն, Բանակցային հմտություններ, Աշխատասիրություն, Բարձրագույն կրթությունը ցանկալի է։ </t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>3/28/2019</t>
+          <t>5/26/2019</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Պահեստապետ</t>
+          <t>Վերապատրաստում և Աշխատանք</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>«Այ Թի Լոջիք» Տեք</t>
+          <t>INECOBANK CJSC</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Accounting, Finance, Banking</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>90000</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t xml:space="preserve">վարորդական իրավունքի առկայություն, տոկունություն,  թիմում աշխատելու կարողություն: </t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>3/28/2019</t>
+          <t>4/25/2019</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Վաճառողուհի / Գանձապահ / Բարիստա</t>
+          <t>Վարկային Մասնագետ</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Sorriso Cafe Gelateria</t>
+          <t>«ՖԻՆՔԱ» ՈՒՎԿ ՓԲԸ</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Sales, Business Development</t>
+          <t>Accounting, Finance, Banking</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Մրցակցային</t>
+          <t>Ashtarak</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ոչ լրիվ աշխատանքային օր Ճկուն գրաֆիկ Աշխատանքային փորձը պարտադիր չէ Ճանապարհածախս Համազգեստ Պաշտոնապես աշխատանքի հաշվառում Կարիերային առաջխաղացման հնարավորություն </t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>3/28/2019</t>
+          <t>5/3/2019</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Ինտերիեր / Էքստերիերի 3D Դիզայներ</t>
+          <t>Business Development Manager</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>3D STUDIO</t>
+          <t>Invest In Network</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Art, Design</t>
+          <t>Sales, Business Development</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Ըստ Պրոեկտի</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Կրթությունը ՝ 3D Vizualizator and Designer,  աշխատանքային փորձ ՝ Պարտադիր, պարտադիր հմտություններ՝ 3Ds Max 2017(18), Corona․ 2 , Photoshope 2017 ծրագրերի գերազանց տիրապետում, ցանկալի հմտություններ՝ 3D Animaciya Interior and Exterior , Vertual Tour 360°: </t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>3/28/2019</t>
+          <t>4/25/2019</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>ՄՌ հավաքագրման մասնագետ /HR Recruiter/</t>
+          <t>Store Manager</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Երեմյան Փրոջեքթս</t>
+          <t>EGO Concept Store</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Human Resources</t>
+          <t>Sales, Business Development</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>3/28/2019</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Հավաքագրման փորձ՝ նվազագույնը 2 տարի,  Հարցազրույց վարելու հմտություն,  Անգլերենի իմացություն աշխատանքային մակարդակում,  Հաղորդակցման հմտություն,  Ուշադրություն և կենտրոնացում: </t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>4/6/2019</t>
+          <t>5/25/2019</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>PHP Ծրագրավորող</t>
+          <t>Front-end Developer</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>ՍՏՌ Արմենիա</t>
+          <t>Innova AM</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -962,168 +807,118 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>3/27/2019</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t xml:space="preserve">HTML- ի եւ CSS- ի լավ իմացություն PHP-ի օգտագործմամբ WEB հավելվածներ մշակելու պրակտիկ փորձ, PHP-ի օգտագործմամբ համակարգերի օբյեկտաուղղորդված նախագծման եւ ծրագրավորման փորձ, PHP-ով ծրագրավորման շրջանակներում jQuery-PHP, JSON, XML եւ AJAX գրադարանների կիրառման միջոցով WEB հավելվածների մշակման փորձ PHP-ի կիրառմամբ (Laravel, Symfony) framework-ների միջոցով ծրագրավորման պրակտիկ փորձ ունենալը տալիս է լրացուցիչ բոնուսներ OOP-ի կիրառմամբ նախագծման և ծրագրավորման ոլորտում խորը գիտելիքներ PHPUnit- ի կիրառման հետ ունեցած աշխատանքային փորձը տալիս է լրացուցիչ բոնուսներ MySQL տվյալների կառավարման համակարգի խորը իմացություն՝ MySQL / PostgreSQL տվյալների կառավարման համակարգերի կիրառմամբ բազաների նախագծման պրակտիկ փորձ LINUX-ի վրա հիմնված օպերացիոն համակարգերի իմացություն, սերվերի վրա ծրագրային համակարգերի տեղակայման եւ սպասարկման ունակություն Google Map-ի տրամադրած միջոցների կիրառման միջոցով ծրագրային համակարգերի մշակման ունակություն PHP- ով համակարգերի մշակման առնվազն 3 տարվա աշխատանքային փորձ սեփական HTTP-API- ի ստեղծման եւ երրորդ կողմի API- ների ինտեգրման փորձ JS-ի կիրառմամբ (jQuery կամ այլ JS framework-ների) կլիենտային մասի ծրագրավորման փորձը կհամարվի էական առավելություն </t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>4/26/2019</t>
+          <t>5/25/2019</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Hardware Designer</t>
+          <t>Թիմ Լիդեր</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>OLYMP Engineering LLC</t>
+          <t>ԷՍԴԻԷՄ</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Information Technologies</t>
+          <t>Sales, Business Development</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>150,000 to 400,000 AMD</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Bachelor's degree in Electronics Engineering or experience in a related field; Experience with PCB Schematics design software’s; Experience working with Altium Designer; Experience designing circuits operating at frequencies greater than 1 GHz; Ability to research and study technical documentation, schematics and datasheets; Demonstrated ability to work in a team environment; Excellent statistical data analysis and problem solving abilities; Basic knowledge in the area of electrical engineering; Knowledge of English language. </t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>3/27/2019</t>
+          <t>5/25/2019</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Հաճախորդների սպասարկման աշխատակից</t>
+          <t>Պրեսելլեր</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>8778 Հայաստան Տեղեկատու</t>
+          <t>ԷՍԴԻԷՄ</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Customer Support, Client Care</t>
+          <t>Sales, Business Development</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>100000 - 120000</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t xml:space="preserve">CorelDrow, Photoshop ծրագրերի իմացությունը պարտադիր QuarkXpress, Adobe Illustrator ծրագերի իմացությամբ ռեզյումեները կդիտարկվեն առաջնային </t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>3/27/2019</t>
+          <t>5/25/2019</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Իրավաբան</t>
+          <t>Արտադրամասի Ղեկավար</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>AM GROUP</t>
+          <t>IMEX GROUP Co. LTD</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Legal, Insurance</t>
+          <t>Production, Operations</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>60,000-500,000դր</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t xml:space="preserve">կրթություն՝ իրավաբան / իրավագետ աշխատանքային փորձը ցանկալի է պարտադիր հմտություններ ՝ համակարգչային գերազանց գիտելիքներ, տրամաբնության և հռետորական արվեստի տիրապետում ցանկալի հմտություններ` օտար լեզվի իմացություն </t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>3/26/2019</t>
+          <t>5/25/2019</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Senior Java Developer</t>
+          <t>Վաճառող</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Catches</t>
+          <t>Մաստեր Գրուպ ՍՊԸ</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Information Technologies</t>
+          <t>Sales, Business Development</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>3/26/2019</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Bachelor's degree in an IT-related field; At least 2 years of experience in Java development; Excellent knowledge of Java Core and OOP; At least 1 year of experience with Spring, Hibernate frameworks, JDBC and Restful API; Strong analytical skills; Advanced/ good level of English language; Knowledge of payment gateways is a big plus. </t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
         <is>
           <t>4/25/2019</t>
         </is>
@@ -1132,49 +927,39 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Արտադրական պրոցեսների ավտոմատացման մասնագետ (АСУТП)</t>
+          <t>Արտադրամասի Վարպետ</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Industrial Components LLC</t>
+          <t>IMEX GROUP Co. LTD</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Engineering</t>
+          <t>Production, Operations</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>3/26/2019</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t xml:space="preserve">տեխնիկական հարցերով խորհրդատվություն հանդիպումներ հաճախորդների հետ ապրանքների և բրենդերի առաջխաղացման նպատակով մասնակցություն դասընթացների և որակավորման բարձրացում նյութերի մշակում և պրեզենտացիաների պատրաստում նոր հաճախորդների ներգրավում </t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>4/25/2019</t>
+          <t>5/25/2019</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Sales Consultant</t>
+          <t>Վաճառքի Մենեջեր</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Թայմլես ՍՊԸ</t>
+          <t>Մեգա Շին ՍՊԸ</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1184,71 +969,51 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>3/25/2019</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Higher education; Work experience in a relevant field is a plus; Fluency in Armenian, Russian and English languages; Good knowledge of MS Excel; knowledge of 1C is a plus; Understanding of the specific of premium product sales; Strong communication and negotiations skills; Highly responsible and attentive to details person; Ability to work under the time pressure. </t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>4/2/2019</t>
+          <t>4/24/2019</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>.NET / .NET Core Software Developers Full Time</t>
+          <t>Տպագրատան Դիզայներ</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Applebrie Limited</t>
+          <t>Ayvazyan &amp; Partners</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Information Technologies</t>
+          <t>Art, Design</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>1,000,000</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t xml:space="preserve">Proven experience as full stack developer Experience working in an Agile Development environment Experience with building web applications/ software Top-notch programming skills and in-depth knowledge of modern code practices Ability to code in a few programming languages (back and front) including Angular, .NET et al. Experience working with web and Rest APIs Solid database experience with MS SQL A solid understanding of how web applications work including security, session management, and best development practices In-depth knowledge of programming for diverse operating systems, browsers and platforms using development tools Excellent understanding of software design and programming principles. A team player with excellent communication skills Analytical thinking and problem-solving capability Great attention to detail and time-management skills BSc/BA in computer science or relevant field Experience in DevOps and SaaS a plus </t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>3/25/2019</t>
+          <t>5/23/2019</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Գլխավոր հաշվապահի օգնական</t>
+          <t>Խնդրահարույց Վարկերի Ավագ Մասնագետ</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ՍՏՌ Արմենիա</t>
+          <t>«ԳԼՈԲԱԼ ԿՐԵԴԻՏ» ՈՒՎԿ ՓԲԸ</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1258,145 +1023,105 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>3/25/2019</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t xml:space="preserve">Բակալավրի աստիճան հաշվապահական հաշվառման, ֆինանսական կամ համապատասխան ոլորտներում 3-5 տարվա աշխատանքային փորձ ՀԾ հաշվապահ 7 ծրագրի իմացություն Հարկային օրենսդրության իմացություն Համակարգչային գիտելիքներ( Word, Excel, PowerPoint, Microsoft project կամ նմանատիպ այլ ծրագիր) Գերազանց վերլուծական հմտություններ Խնդիրների լուծման և որոշումներ կայացնելու խորը զարգացած հմտություններ Պլանավորման և կազմակերպչական հմտություններ, Համագործակցում/թիմային աշխատանք Գերազանց հայերեն, ռուսերեն լեզուների իմացություն, անգլերերենի իամցությունը ցանկալի </t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>4/24/2019</t>
+          <t>4/23/2019</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Բանվոր - Առաքիչ</t>
+          <t>Beauty Salon Administrator</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ՅՈՒՆԻՓՈՒԼ ՍՊԸ</t>
+          <t>10 nails bar</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Customer Support, Client Care</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>130,000 ՀՀդրամ+պարգևատրում</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t xml:space="preserve">կրթություն - միջնակարգ աշխատանքային փորձ  պարտադիր հմտություններ - մեքենայի վարում B կարգ </t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>3/22/2019</t>
+          <t>5/23/2019</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Տեղեկատվական Կենտրոնի Աշխատակցուհի</t>
+          <t>DevOps Engineer</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>ՄԵԾ ԱՆԻՎ</t>
+          <t>Innova AM</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Administrative, Clerical</t>
+          <t>Information Technologies</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>3/22/2019</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t xml:space="preserve">Բարձրագույն կրթություն, Հայերեն, ռուսերեն  և անգլերեն լեզուների գերազանց իմացություն,  Հաղորդակցման բարձր հմտություններ, Բարեհամբույր, Կոնֆլիկտային իրավիճակներում կողմնորոշվելու ունակություն, Համակարգչային գիտելիքներ, Photoshop կամ Corel Draw ծրագրերի պարտադիր իմացություն: </t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>4/21/2019</t>
+          <t>4/23/2019</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Ներգնա Տուր Մենեջեր</t>
+          <t>Բարիստա Մատուցող</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Aquarius Travel</t>
+          <t>Opera Suite Hotel</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Tourism, Hospitality</t>
+          <t>Restaurants, Food Services</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>3/22/2019</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t xml:space="preserve">Պարտադիր հմտություններ՝ լեզուների ԳԵՐԱԶԱՆՑ իմացություն Համակարգչային՝ Microsoft ծրագրերի գերազանց տիրապետում աշխատանքային փորձը պարտադիր չէ ցանկալի հմտություններ՝ ակտիվ, շփվող, արագ ըմբռնող, լավ հիշողություն </t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>4/21/2019</t>
+          <t>5/23/2019</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Շուկայի Զարգացման Պատասխանատու</t>
+          <t>Վաճառքի Մենեջեր</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Ayvazyan &amp; Partners</t>
+          <t>Վանիթար</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1406,34 +1131,24 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>մրցակցային բարձր</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t xml:space="preserve">Բարձրագույն կրթություն Առնվազն 2 տարվա աշխատանքային փորձ վաճառքի ոլորտում Հաղորդակցման և բանակցելու գերազանց հմտություններ MS Office փաթեթի լավ իմացություն,1C-ի իմացությունը կդիտվի որպես առավելություն Ճկունություն և սթրեսակայունություն Մեծ ծավալի տեղեկատվության հետ աշխատելու ունակություն Ինքնակատարելագուրծման մեծ ցանկություն և պատասխանատվություն </t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>3/22/2019</t>
+          <t>5/23/2019</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Վաճառքի Մենեջեր</t>
+          <t>International Sales Manager</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Մոշն Թայմ</t>
+          <t>00194051</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1443,34 +1158,24 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>3/22/2019</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t xml:space="preserve">բարձրագույն կրթություն (ցանկալի է տնտեսագիտության ոլորտում) աշխատանքային փորձ առնվազն 1 տարի հայերեն գրագետ բանավոր և գրավոր խոսք, ռուսերենի և անգլերենի գերազանց իմացությունը կդիտվի որպես առավելություն համակարգչային գիտելիքներ - Microsoft Office, Microsoft Excel, Power Point մեծ ծավալի տեղեկատվության հետ աշխատելու ունակություն սթրեսակայունություն </t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>4/21/2019</t>
+          <t>4/23/2019</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Մարքեթինգի Մենեջեր</t>
+          <t>Մարքեթինգի Մասնագետ</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Մոշն Թայմ</t>
+          <t>IMEX GROUP Co. LTD</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1480,737 +1185,537 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>3/21/2019</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t xml:space="preserve">Բարձրագույն կրթություն մարքեթինգի կամ բիզնեսի կառավարման ոլորտում, Համապատասխան ոլորտում աշխատանքային փորձ, Սոցիալական կայք - էջերի վարման փորձառություն, կայքի օպտիմիզացիա և առաջխաղացում SEO գործիքների բազային իմացություն, ինչպիսին են Google Analytics, Google Adwords, Webmaster, HTML, CSS Facebook, Twitter, Instagram, Tumblr, Youtube, Pinterest, Linkedin, Google+ լավ իմացություն, Վաճառքների խթանման փորձ, Հաղորդակցության գերազանց հմտություններ, Նորարար և կրեատիվ մտածողություն, Վերլուծական մտածողություն, Նախագծերի կառավարման ունակություն, Թիմում աշխատելու հմտություններ, Հայերեն, անգլերեն և ռուսերեն լեզուների իմացություն, Microsoft Office ծրագրերի լավ իմացություն, Տպարանների, դիզայն ստուդիաների և աշխատանքի համար անհրաժեշտ նյութերի մատակարարների հետ աշխատելու փորձ: </t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>4/20/2019</t>
+          <t>5/23/2019</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Գրաֆիկ Դիզայներ</t>
+          <t>Մարքեթինգի Մասնագետ</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Մոշն Թայմ</t>
+          <t>Lesona LLC</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Art, Design</t>
+          <t>Marketing, Advertising, PR</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>3/21/2019</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t xml:space="preserve">Կրեատիվ և հետաքրքիր մտածողություն Ֆանտազիայի առկայություն Adobe Photoshop, Adobe Illustrator/Corel Draw և 3ds Max-ի պարտադիր իմացություն Թիմում աշխատելու կարողություն և պատրաստակամություն Լարված իրավիճակներում աշխատելու կարողություն Հստակ վերջնաժամկետների պայմաններում աշխատելու կարողություն և պատասխանատվություն </t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>4/20/2019</t>
+          <t>5/23/2019</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Գանձապահ</t>
+          <t>Sales Manager</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Mr. GYROS</t>
+          <t>Bass Boutique Hotel</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Accounting, Finance, Banking</t>
+          <t>Sales, Business Development</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>3/21/2019</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t xml:space="preserve">POS, ՀԴՄ-ի հետ աշխատելու կարողություն, Դրամական միջոցների հետ աշխատելու կարողություն, Հստակ ձեւակերպված պարզ խոսք (ռուսերեն, անգլերեն մինիմալ գիտելիքներ), Թիմային աշխատանքի ցանկություն եւ կարողություն, Արագ կողմնորոշվելու ունակություն, զարգացած ուշադրություն եւ հիշողություն, Պարտաճանաչություն, պատասխանատվության բարձր զգացում: </t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>4/20/2019</t>
+          <t>4/22/2019</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Տուրիզմի Մենեջեր</t>
+          <t>Կորպորատիվ Վաճառքի Մասնագետ</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Maratuk LLC</t>
+          <t>FNet</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Tourism, Hospitality</t>
+          <t>Sales, Business Development</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>3/20/2019</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t xml:space="preserve">Բարձրագույն կրթություն, Աշխատանքային փորձ տուրիզմի բնագավառում, Անգլերեն և ռուսերեն լեզուների վարժիմացություն, արաբերենի բավարար իմացություն, MS Office ծրագրերի իմացություն, Հաղորդակցվելու ունակություն, ճկունություն, Թիմային աշխատանք: </t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>Դուբայ ԱՄԷ</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>4/19/2019</t>
+          <t>4/30/2019</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Վաճառքի Մենեջեր</t>
+          <t>Մարքեթինգի Պատասխանատու</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>ՍՏՌ Արմենիա</t>
+          <t>«Այ Թի Լոջիք» Տեք</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Sales, Business Development</t>
+          <t>Marketing, Advertising, PR</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>3/20/2019</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t xml:space="preserve">աշխատանքային փորձը վաճառքի ոլորտում ցանկալի է լեզվական հմտություններ. հայերեն, ռուսերեն և անգլերեն լեզուների իմացություն, համկարգչային ծրագրերի տիրապետում (MS  office  Word, Excel) արդյունավետ թիմային աշխատանքի և ժամանակի կառավարման հմտություններ, կազմակերպչական, հաղորդակցման և բանակցությունների վարման հմտություններ,  կոնֆլիկտների և սթրեսային իրավիճակների կառավարման հմտություններ։ </t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>4/19/2019</t>
+          <t>4/22/2019</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Թիմ Լիդեր</t>
+          <t>Խոհարար</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Տիկո Հոլդինգ ՍՊԸ</t>
+          <t>Mr. GYROS</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Sales, Business Development</t>
+          <t>Restaurants, Food Services</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Պայմանագրային</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t xml:space="preserve">Աշխատանքային փորձը պարտադիր է, Ավտոմեքենայի առկայությունը պարտադիր է: </t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>3/20/2019</t>
+          <t>5/22/2019</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Բարմեն - Բարիստա</t>
+          <t>Վաճառքի Տնօրեն</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Sorriso Cafe Gelateria</t>
+          <t>Ayvazyan &amp; Partners</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Restaurants, Food Services</t>
+          <t>Project, Program Management</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>200000</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ոչ լրիվ աշխատանքային օր Ուսուցում Ճկուն գրաֆիկ Ճանապարհածախս Համազգեստ Պաշտոնապես աշխատանքի հաշվառում Կարիերային առաջխաղացման հնարավորություն </t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>3/20/2019</t>
+          <t>5/22/2019</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Ռեստորանի Մենեջեր</t>
+          <t>Վաճառքի Մենեջեր</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Yasaman Family LLC</t>
+          <t>Ayvazyan &amp; Partners</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Restaurants, Food Services</t>
+          <t>Sales, Business Development</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>3/19/2019</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t xml:space="preserve">Տարիք՝ 25-35, Բարձրագույն կրթությունը և աշխատանքային փորձը ռեստորանային ոլորտում կդիտվի որպես առավելություն, Ռուսերեն և անգլերեն լեզվի իմացությունը կդիտվի որպես առավելություն, Ղեկավարման փորձ՝ 1-3տ., Ներկայանալի տեսք, Հաղորդակցման ունակություն և բարդ իրավիճակներում մարդկանց հետ շփվելու կարողություն, Ուղղորդման ունակություն և կազմակերպչական հմտություններ, Պատասխանատվության զգացում և աշխատանքի նկատմամբ բարեխիղճ վերաբերմունք, Արագ կողմնորոշվելու, ինքնուրույն որոշումներ կայացնելու ունակություն, մտքի և վարքի ճկունություն, Ժպտերես, բարեհամբյուր: </t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>4/18/2019</t>
+          <t>5/22/2019</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Contact Center Specialist</t>
+          <t>Տպագրիչ</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>DIGITAIN</t>
+          <t>Ayvazyan &amp; Partners</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Customer Support, Client Care</t>
+          <t>Production, Operations</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>3/19/2019</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t xml:space="preserve">A natural communicator Confident and can-do, with a natural ability to deliver an excellent customer service Proficient in Armenian, Russian and English languages (written and verbal) With good knowledge of MS Office (Word, Excel) will be an asset Responsible Able to work under pressure </t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>4/18/2019</t>
+          <t>5/22/2019</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Ադմինիստրատոր</t>
+          <t>Ճարտարապետ - Դիզայներ</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>«ԲիԷսԹի» ՍՊԸ</t>
+          <t>Albedo Graphics LLC</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Administrative, Clerical</t>
+          <t>Art, Design</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>130000</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t xml:space="preserve">բարձրագույն կրթությունը`ցանկալի է տնտեսագիտական կամ տեխնիկական աշխատանքային փորձը պարտադիր է MS Office-ի լավ իմացություն Օտար լեզուների (ռուսերեն, անգլերեն) իմացությունը ցանկալի է Տարիքը՝ 25-45 տարեկան Սեռը՝ իգական  </t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>3/19/2019</t>
+          <t>4/20/2019</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Տուր Օպերատոր</t>
+          <t>Մատուցող / Մատուցողուհի</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Best Tour</t>
+          <t>“HMG“ ընկերություն</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Tourism, Hospitality</t>
+          <t>Restaurants, Food Services</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>90000</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t xml:space="preserve">Բարձրագույն կրթություն Զբոսաշրջային ուղղությունների տիրապետում Տուրիստական փաթեթներ կազմելու և վաճառելու հմտություն Կազմակերպված, պատասխանատու, աշխատասեր Համակարգչային Գիտելիքներ Հայերենի, անգլերենի և ռուսերենի գերազանց իմացություն Գրագետ բանավոր և գրավոր խոսք Աշխատանքային փորձը ցանկալի է </t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>3/18/2019</t>
+          <t>4/19/2019</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Java Developer</t>
+          <t>Վաճառքի Պատասխանատու</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Technology and Science Dynamics LLC</t>
+          <t>IMEX GROUP Co. LTD</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Information Technologies</t>
+          <t>Customer Support, Client Care</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>3/18/2019</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t xml:space="preserve">An experience of at least 5+ years in the development of Java applications;  An experience of at least 5+ years with each of the following technologies: HTML, XML, CSS, JavaScript;  An experience of at least 5 years with: Vaadin;  An experience of at least 5+ years with each of the following technologies: Spring, Hibernate, SQL;  An experience of at least 5+ years with the following technology: Web Services with SOAP;  An experience of at least 5+ years with each of the following technologies: A continuous integration tool like Jenkins, Hudson, Maven, Subversion. </t>
-        </is>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>4/17/2019</t>
+          <t>5/19/2019</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Ինժեներ - Էլեկտրոնշիկ</t>
+          <t>Սպասարկող Մենեջեր</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>NewPlast CJSC</t>
+          <t>IMEX GROUP Co. LTD</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Engineering</t>
+          <t>Customer Support, Client Care</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>3/18/2019</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t xml:space="preserve">Բարձրագույն կրթություն  Անգլերեն լեզվի իմացություն  Աշխատանքային փորձը համապատասխան ոլորտում պարտադիր է  Արագ կողմնորոշվելու, ճկուն և ճշգրիտ աշխատելու ունակություն  Մանրուքների նկատմամբ ուշադրություն, կարգապահություն և պատասխանատվության զգացում  Աշխատանքը համակարգելու ունակություն  Թիմում աշխատելու ունակություն  Ինֆորմացիայի ընկալման կարողություն  Մինիմալ հսկողության պայմաններում աշխատելու ունակություն  Պարտաճանաչություն, ճշտապահություն աշխատանքը անթերի իրականացնելու ունակություն </t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>4/22/2019</t>
+          <t>5/19/2019</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Մաքրության պատասխանատու</t>
+          <t>1C համակարգի ծրագրավորող</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>GIFT CITY</t>
+          <t>IMEX GROUP Co. LTD</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Information Technologies</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>100000</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t xml:space="preserve">աշխատանքային փորձ բարեխիղճ պատասխանատու պունկտուալ արագաշարժ աշխատասեր մաքրասեր ճշտախոս </t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>3/18/2019</t>
+          <t>5/19/2019</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Գրասենյակի աշխատակից</t>
+          <t>Սերտիֆիկացման / Ստանդարտացման մասնագետ</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Արագած Ֆուդ</t>
+          <t>Տոնուս - Լես</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Administrative, Clerical</t>
+          <t>Medical, Health, Fitness, Beauty</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>3/15/2019</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t xml:space="preserve">աշխատանքային փորձը ցանկալի է համակարգչային գիտելիքներ ճշտապահ նպատակասլաց </t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>4/14/2019</t>
+          <t>5/18/2019</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Խորհրդատու - Վաճառող</t>
+          <t>Փաստաբան / Իրավաբան</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Lesona LLC</t>
+          <t>02538904</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Sales, Business Development</t>
+          <t>Legal, Insurance</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>3/15/2019</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t xml:space="preserve">Բարձրագույն կրթություն Սպասարկման ոլորտում աշխատանքային փորձ Ռուսերեն և անգլերեն լեզուների իմացություն Համակարգչային բազային գիտելիքներ Հաղորդակցման և թիմային աշխատանքի հմտություններ Ճշտապահություն և պատասխանատվության զգացում </t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>4/14/2019</t>
+          <t>4/18/2019</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Հաշվապահ</t>
+          <t>Էլեկտրիկ</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Սեմուր ընդ Կո ՍՊԸ</t>
+          <t>Մեգա Շին ՍՊԸ</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Accounting, Finance, Banking</t>
+          <t>Engineering</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>3/14/2019</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t xml:space="preserve">բարձրագույն կրթություն (ցանկալի է մասնագիտական կամ տեխնիկական) աշխատանքային փորձ՝ առնվազն 1 տարի պարտադիր հմտություններ՝ հաշվային պլան, ՀԾ-հաշվապահ 7, Excel ցանկալի հմտություններ՝ e-Invoicing, Microsoft Office աշխատասիրություն, աշխատանքի նկատմամբ պատասխանատվություն, թիմում աշխատելու ունակություն </t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>4/13/2019</t>
+          <t>4/17/2019</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Պրեսելլեր</t>
+          <t>Վարորդ Առաքիչ</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>ԷՍԴԻԷՄ</t>
+          <t>Մեգա Շին ՍՊԸ</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Sales, Business Development</t>
+          <t>Logistics, Transportation</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>3/13/2019</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t xml:space="preserve">Բարձրագույն կրթություն Աշխատանքային փորձը տվյալ ոլորտում պարտադիր է Մեքենայի առկայությունը պարտադիր է </t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>4/12/2019</t>
+          <t>4/17/2019</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Թիմ Լիդեր</t>
+          <t>Administrative Assistant</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ԷՍԴԻԷՄ</t>
+          <t>Innova AM</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Sales, Business Development</t>
+          <t>Administrative, Clerical</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>3/13/2019</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t xml:space="preserve">Բարձրագույն կրթություն տնտեսագիտության ոլորտում, հայերեն և ռուսերեն լեզուների իմացություն, համակարգչի տիրապետում: աշխատանքային փորձը  պարտադիր է:  </t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>4/12/2019</t>
+          <t>4/17/2019</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Պիցցայի Մասնագետ</t>
+          <t>Technical Writer</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>The LOFT</t>
+          <t>Pay&amp;Go</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Restaurants, Food Services</t>
+          <t>Information Technologies</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>3/12/2019</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t xml:space="preserve">Պատրաստել պիցցաներ (տարբեր բաղադրիչներով) Պատրաստել կարկանդակներ (տարբեր միջուկներով ) Պատրաստել լանչեր (*քննարկման ենթակա) </t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>4/11/2019</t>
+          <t>5/16/2019</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Շուկայի Զարգացման Պատասխանատու</t>
+          <t>Խորհրդատու Վաճառող</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Սիկոնե ՍՊԸ</t>
+          <t>Lesona LLC</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2220,108 +1725,78 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>200,000</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ապահովել ներկայացված ապրանքների ԱՌԱՋԱՏԱՐ ԴԻՐՔԵՐԸ Ներկայացնել և վաճառել ներկայացվող ապրանքները Պահպանել հին գործընկերների լոյալությունը, Ուսումնասիրել շուկան, գտնել նոր գործընկերներ, Հետևել խանութներում ապրանքների տեսակների առկայությանը, (դասավորվածությանը, գնապիտակների առկայուրյունն ու ճշտությանը), տեսանելիությանը </t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>3/11/2019</t>
+          <t>5/16/2019</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Գլխավոր Հաշվապահ</t>
+          <t>Մատուցող / Մատուցողուհի</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Հայաստանի Աստվածաշնչային Ընկերություն</t>
+          <t>Figaro LLC</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Accounting, Finance, Banking</t>
+          <t>Restaurants, Food Services</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>300,000՝ ներառյալ հարկերը</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t xml:space="preserve">բարձրագույն կրթություն ՀԾ հաշվապահական ծրագիրի իմացություն անգլերենի և ռուսերենի լավ իմացություն </t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>3/11/2019</t>
+          <t>4/16/2019</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Գանձապահ / Ադմինիստրատոր</t>
+          <t>ՄՌԿ Օգնական</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Beer Academy</t>
+          <t>Mr. GYROS</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Restaurants, Food Services</t>
+          <t>Human Resources</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>120000</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t xml:space="preserve">լինել ժպտերես սովորել ռեստորանային ծրագիրը </t>
-        </is>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>3/11/2019</t>
+          <t>5/16/2019</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Front-End Developer (Mid Level)</t>
+          <t>Full Stack CTO</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Concept Studio</t>
+          <t>Raleigh &amp; Drake</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2331,108 +1806,78 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>3/11/2019</t>
+          <t>Los Angeles, CA</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t xml:space="preserve">Expert level skills in HTML, CSS and JavaScript Experience with React, other JavaScript frameworks is a bonus Experience working with CMSs Hands on experience with the following: SASS/SCSS GIT Experience with less or sass frameworks Experience in using Canvas or tweenMax is a plus Solid command of responsive layouts 2+ years of working in the tech industry Testing experience (a plus) Understanding of cross-browser compatibility issues and ways to work around them Zero intimidation of new technologies and ability to self-teach quickly yourself on the fly Ability to communicate positively and honestly Strong work ethic and reliability </t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>4/10/2019</t>
+          <t>4/15/2019</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Սննդամթերքի որակի և անվտանգության մասնագետ</t>
+          <t>.NET Developer</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Ա/Ձ Իննա Կոջոյան</t>
+          <t>Pay&amp;Go</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Administrative, Clerical</t>
+          <t>Information Technologies</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Պայմանագրային</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t xml:space="preserve">բարձրագույն կրթություն` ցանկալի է բժշկական, գյուղատնտեսության, կենսաբանության ոլորտներում հայերեն լեզվի գերազանց, ռուսերեն և անգլերեն լեզուների լավ իմացություն համակարգչային գիտելիքներ (MS Office) աշխատանքային փորձը ցանկալի է պատասխանատվության բարձր զգացում հաղորդակցվելու գերազանց  ունակություն նոր գիտելիքներ և հմտություններ ձեռք բերելու մշտական ցանկություն </t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>3/7/2019</t>
+          <t>5/15/2019</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Վաճառքի մենեջեր</t>
+          <t>Որակի Հսկողության Բաժնի Ղեկավար</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Մեգա Շին ՍՊԸ</t>
+          <t>«Գլորիա» Կարի Ֆաբրիկա</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Sales, Business Development</t>
+          <t>Production, Operations</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>բարձր</t>
+          <t>Vanadzor</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t xml:space="preserve">Հաղորդակցման գերազանց հմտություններ, կիրթ խոսելաոճ Պատասխանատու և պարտաճանաչ մոտեցում աշխատանքին Շինանյութի վաճառքների ոլորտում առնվազն 2 տարվա աշխատանքային փորձ Ռուսերեն լեզվի իմացությունը պարտադիր է </t>
-        </is>
-      </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>3/6/2019</t>
+          <t>4/12/2019</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Լոգիստիկայի և Ներմուծման Մենեջեր</t>
+          <t>Վարորդ</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Մեգա Շին ՍՊԸ</t>
+          <t>Brand Leader</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2442,108 +1887,78 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>120000+bonus</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ռուսերեն լեզվի գրավոր և բանավոր իմացությունը պարտադիր է Համակարգչից վարժ օգտվելը պարտադիր է Անգլերեն լեզվի իմացությունը ցանկալի է Աշխատանքային փորձը ներմուծման ոլորտում պարտադիր է </t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>3/6/2019</t>
+          <t>4/12/2019</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Արտադրության Տնօրեն</t>
+          <t>Անձնական Վարորդ</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Մեգա Շին ՍՊԸ</t>
+          <t>Trapezza</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Production, Operations</t>
+          <t>Logistics, Transportation</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>120000+bonus</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t xml:space="preserve">Արտադրության կազմակերպման և ղեկավարման ոլորտում 3 տարվա փորձը պարտադիր է, շինանյութի ոլորտում՝ ցանկալի ինժեներական կրթությունը ցանկալի է մեխանիկայից, էլեկտրիկայից, հիդրավլիկայից մինիմալ գիտելիքներ </t>
-        </is>
-      </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>3/6/2019</t>
+          <t>4/12/2019</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Բժշկական Ներկայացուցիչ</t>
+          <t>Խանութ - Սրահի Մենեջեր</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>RECORDATI</t>
+          <t>"Մաքուր Տուն" ՍՊԸ</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Medical, Health, Fitness, Beauty</t>
+          <t>Sales, Business Development</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>3/6/2019</t>
+          <t>Abovyan</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t xml:space="preserve">բարձրագույն մասնագիտական կրթություն լեզուների իմացություն. հայերեն, ռուսերեն՝ գերազանց, անգլերենի իմացույթունը կդիտվի որպես  առավելություն համակարգչային գրագիտություն (MS office) թիմում աշխատելու ունակություն բանակցություններ վարելու ունակություն վարորդական իրավունք (մեքենա վարելու փորձը ցանկալի է) անձնային հատկություններ. շփվող, նպատակասլաց, նախաձեռնող, պատասխանատու աշխատանքային փորձը ցանկալի է  </t>
-        </is>
-      </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>4/5/2019</t>
+          <t>5/12/2019</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Վաճառքի Մասնագետ</t>
+          <t>Ցանցի զարգացման մասնագետ</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>ԻՆԳՈ ԱՐՄԵՆԻԱ ԱՓԲԸ</t>
+          <t>"Մաքուր Տուն" ՍՊԸ</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2553,251 +1968,181 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>3/6/2019</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t xml:space="preserve">Բարձրագույն կրթություն Վաճառքի հմտություններ Առաջնորդի հատկանիշներ MS Excel ծրագրի փայլուն իմացություն Առնվազն երեք լեզվի իմացություն (հայերեն, ռուսերեն և անգլերեն) Համակարգչային տեքստերի մուտքագրման ունակություն Սովորելու, արագ յուրացնելու ընդունակություն և պատրաստակամություն Նամակագրության էթիկայի հմտություններ </t>
-        </is>
-      </c>
-      <c r="F60" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>4/5/2019</t>
+          <t>5/12/2019</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Pet Groomer</t>
+          <t>Խանութ - Սրահի Մենեջեր</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Wejeco Pet Hotel</t>
+          <t>"Մաքուր Տուն" ՍՊԸ</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Medical, Health, Fitness, Beauty</t>
+          <t>Sales, Business Development</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>3/5/2019</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t xml:space="preserve">Compassion: Dogs and cats often get stressed out in unfamiliar situations, and groomers need to understand this and treat them accordingly. Customer-Service: Groomers work with customers directly, and must be friendly and listen to their requests and needs. Attention to Detail: Groomers must pay attention to what they are doing so that the animals stay safe and the grooming comes out looking great. Stamina: Groomers are on their feet for long periods of time, sometimes hunched over animals during the grooming process. Fluency in English and Armenian, any additional languages is a plus Proven ability to follow instructions and learn new things Ability to work in a team environment </t>
-        </is>
-      </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>4/4/2019</t>
+          <t>5/12/2019</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Կադրերի Բաժնի Վարիչ / Իրավաբան</t>
+          <t>Վաճառքի Մենեջեր</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>ՀՀ ԳԱԱ Հայկենսատեխնոլոգիա ԳԱԿ ՊՈԱԿ</t>
+          <t>Medtechservice LLC</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Human Resources</t>
+          <t>Sales, Business Development</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>3/5/2019</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t xml:space="preserve">կրթություն՝ բարձրագույն իրավաբանական աշխատանքային փորձ՝ պարտադիր պարտադիր հմտություններ՝ համակարգչային ծրագրեր, օտար լեզվուների իմացություն՝ ռուսերեն, անգլերեն </t>
-        </is>
-      </c>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>4/4/2019</t>
+          <t>5/12/2019</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Էլեկտրոմեխանիկ</t>
+          <t>Արտաքին Կապերի Մասնագետ</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>«Այ Թի Լոջիք» Տեք</t>
+          <t>Union of Communities of Armenia</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Engineering</t>
+          <t>Marketing, Advertising, PR</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>3/5/2019</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t xml:space="preserve">30-45տ  ունենալ միջին մասնագիտական կրթություն ունենալ աշխատանքային փորձ ունենալ պատասխանատվության բարձր զգացում </t>
-        </is>
-      </c>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>4/4/2019</t>
+          <t>5/11/2019</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Freight Broker</t>
+          <t>B2B Sales Manager</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Momentum</t>
+          <t>Lanar Service LLC</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Logistics, Transportation</t>
+          <t>Sales, Business Development</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>3/4/2019</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t xml:space="preserve">Fluent English is required Spanish is an asset Good listening and speaking skills in English (advanced level) Good communication skills Assidious and orderly personality </t>
-        </is>
-      </c>
-      <c r="F64" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>4/3/2019</t>
+          <t>5/11/2019</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Մատուցող / Մատուցողուհի</t>
+          <t>Platform Administration Specialist</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Figaro LLC</t>
+          <t xml:space="preserve">SEF International UCO </t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Customer Support, Client Care</t>
+          <t>Information Technologies</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>180000 և ավել</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t xml:space="preserve">դիմավորել և ճանապարհել հյուրերին ու այցելուներին լինել ժպտերես հաճախորդամետ բարեհամբյուր նրբանկատ ուշադիր </t>
-        </is>
-      </c>
-      <c r="F65" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>3/4/2019</t>
+          <t>5/10/2019</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Ավագ Խոհարար</t>
+          <t>Ծրագրերի և ֆոնդհայթայթման պատասխանատու</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Figaro LLC</t>
+          <t>Union of Communities of Armenia</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Restaurants, Food Services</t>
+          <t>Administrative, Clerical</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>500000</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t xml:space="preserve">կրթությունը ցանկալի է  աշխատանքային փորձը եվրոպական խոհանոցում պարտադիր է  </t>
-        </is>
-      </c>
-      <c r="F66" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>3/4/2019</t>
+          <t>5/10/2019</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Գլխավոր Հաշվապահ</t>
+          <t>Վաճառքի Բաժնի Տնօրեն</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2807,39 +2152,29 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Accounting, Finance, Banking</t>
+          <t>Sales, Business Development</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>3/4/2019</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t xml:space="preserve">Արտոնագրված մասնագետ (պարտադիր), Բակալավրի աստիճան հաշվապահական հաշվառման, ֆինանսական կամ համապատասխան ոլորտներում, Առնվազն 5 տարվա աշխատանքային փորձ միջինում 2 միլիարդ շրջանառություն ունեցող ընկերությունում, Գրավոր հաշվետվությունների կազմման հմտություններ, 1С ծրագրի գերազանց իմացություն, Համակարգչային գիտելիքներ( ՀԾ, Word, Excel, PowerPoint, Microsoft project կամնմանատիպ այլ ծրագիր), Գերազանց վերլուծական հմտություններ, Խնդիրների լուծման և որոշումներ կայացնելու խորը զարգացած հմտություններ, Կառավարման հմտություններ, Պլանավորման և կազմակերպչական հմտություններ, Համագործակցում/թիմային աշխատանք, Գերազանց հայերեն, ռուսերեն լեզուների իմացություն, անգլերերենի իամցությունը` ցանկալի: </t>
-        </is>
-      </c>
-      <c r="F67" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>4/3/2019</t>
+          <t>5/10/2019</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Վաճառքի Մասնագետ</t>
+          <t>Վաճառքի Մենեջեր</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Narplast LLC</t>
+          <t>Տիկո Հոլդինգ ՍՊԸ</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2849,91 +2184,228 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>170000-200000</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t xml:space="preserve">Բարձրագույն կրթություն Աշխատանքային փորձ`որպես վաճառքի մասնագետ Հայերեն լեզվի կատարյալ իմացություն (ռուսերենի և անգլերենի իմացությունը ցանկալի է) Հաղորդակցվելու գերազանց ունակություն Համակարգչային գիտելիքներ` Word, Excel, 1C Ճկունություն և թիմում աշխատելու ունակություն </t>
-        </is>
-      </c>
-      <c r="F68" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G68" t="inlineStr">
-        <is>
-          <t>2/26/2019</t>
+          <t>5/10/2019</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Շուկայի Զարգացման Պատասխանատու</t>
+          <t>Եռակցման մասնագետ / Специалист по сварке</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Մաստեր Գրուպ ՍՊԸ</t>
+          <t>GeoProMining Gold LLC</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Sales, Business Development</t>
+          <t>Engineering</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>2/26/2019</t>
+          <t>Vardenis</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t xml:space="preserve">բարձրագույն կրթություն աշխատանքային փորձը ցանկալի է հայերեն, ռուսերեն լեզվի գրագետ խոսք, անգլերենի  իմացությունը կդիտվի որպես առավելություն համակարգչային գիտելիքներ պատասխանատվության բարձր զգացում հաղորդակցվելու գերազանց  ունակություն </t>
-        </is>
-      </c>
-      <c r="F69" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>4/2/2019</t>
+          <t>4/9/2019</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Technical Sales and Customer Support Agent</t>
+          <t>Հաշվապահ</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Piconet</t>
+          <t>ՄԵԾ ԱՆԻՎ</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Customer Support, Client Care</t>
+          <t>Accounting, Finance, Banking</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>200.000</t>
-        </is>
-      </c>
-      <c r="F70" t="inlineStr">
-        <is>
-          <t>Yerevan</t>
-        </is>
-      </c>
-      <c r="G70" t="inlineStr">
-        <is>
-          <t>2/25/2019</t>
+          <t>Yerevan</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>5/9/2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Շուկայի Զարգացման Պատասխանատու (Պրեսելլեր)</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Brand Leader</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Sales, Business Development</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Yerevan</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>4/9/2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Վաճառող - Խորհրդատու</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Sacvoyage store</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Sales, Business Development</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Yerevan</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>5/9/2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Մատուցող / Մատուցողուհի</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Classic Burger</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Restaurants, Food Services</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Yerevan</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>5/14/2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Սանտեխնիկ</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Նոր Երևան</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Yerevan</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>4/8/2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Էներգետիկ</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Նոր Երևան</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Yerevan</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>4/8/2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Ռեստորանի Աշխատակից</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>"FASTFOOD" KFC</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Restaurants, Food Services</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Yerevan</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>4/8/2019</t>
         </is>
       </c>
     </row>

</xml_diff>